<commit_message>
updated file names for GA workflow
</commit_message>
<xml_diff>
--- a/group-accounts/ebd_users_GA_relSep-2021.xlsx
+++ b/group-accounts/ebd_users_GA_relSep-2021.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCI\ebird-datasets\group-accounts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCI\covid-ebirding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7A2192E4-D307-4FDB-9976-4007EDF5CE34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA4CCD3-3E2F-45FE-9129-77088A506BD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ebd_users_GA_relSep-2021" sheetId="1" r:id="rId1"/>
     <sheet name="ReadMe" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -2504,7 +2504,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3053,17 +3053,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3383,11 +3373,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3395,11 +3385,10 @@
     <col min="1" max="1" width="5.77734375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="58.109375" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="5"/>
-    <col min="6" max="6" width="63.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="63.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>800</v>
       </c>
@@ -3475,6 +3464,7 @@
       <c r="E4" s="5">
         <v>1</v>
       </c>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -3492,6 +3482,7 @@
       <c r="E5" s="5">
         <v>1</v>
       </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -3509,6 +3500,7 @@
       <c r="E6" s="5">
         <v>1</v>
       </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -3546,6 +3538,7 @@
       <c r="E8" s="5">
         <v>1</v>
       </c>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -3563,6 +3556,7 @@
       <c r="E9" s="5">
         <v>0</v>
       </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -3580,6 +3574,7 @@
       <c r="E10" s="5">
         <v>1</v>
       </c>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -3597,6 +3592,7 @@
       <c r="E11" s="5">
         <v>1</v>
       </c>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -3614,6 +3610,7 @@
       <c r="E12" s="5">
         <v>0</v>
       </c>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -3651,6 +3648,7 @@
       <c r="E14" s="5">
         <v>0</v>
       </c>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -3708,6 +3706,7 @@
       <c r="E17" s="5">
         <v>1</v>
       </c>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -3725,6 +3724,7 @@
       <c r="E18" s="5">
         <v>1</v>
       </c>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -3742,6 +3742,7 @@
       <c r="E19" s="5">
         <v>1</v>
       </c>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -3759,6 +3760,7 @@
       <c r="E20" s="5">
         <v>1</v>
       </c>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -3776,6 +3778,7 @@
       <c r="E21" s="5">
         <v>1</v>
       </c>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -3793,6 +3796,7 @@
       <c r="E22" s="5">
         <v>0</v>
       </c>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -3890,6 +3894,7 @@
       <c r="E27" s="5">
         <v>0</v>
       </c>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -3907,6 +3912,7 @@
       <c r="E28" s="5">
         <v>0</v>
       </c>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -3924,6 +3930,7 @@
       <c r="E29" s="5">
         <v>1</v>
       </c>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -3981,6 +3988,7 @@
       <c r="E32" s="5">
         <v>0</v>
       </c>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
@@ -3998,6 +4006,7 @@
       <c r="E33" s="5">
         <v>1</v>
       </c>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -4015,6 +4024,7 @@
       <c r="E34" s="5">
         <v>1</v>
       </c>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -4032,6 +4042,7 @@
       <c r="E35" s="5">
         <v>0</v>
       </c>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -4069,6 +4080,7 @@
       <c r="E37" s="5">
         <v>0</v>
       </c>
+      <c r="F37" s="6"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -4086,6 +4098,7 @@
       <c r="E38" s="5">
         <v>0</v>
       </c>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
@@ -4103,6 +4116,7 @@
       <c r="E39" s="5">
         <v>0</v>
       </c>
+      <c r="F39" s="6"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -4120,6 +4134,7 @@
       <c r="E40" s="5">
         <v>0</v>
       </c>
+      <c r="F40" s="6"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -4137,6 +4152,7 @@
       <c r="E41" s="5">
         <v>0</v>
       </c>
+      <c r="F41" s="6"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
@@ -4194,6 +4210,7 @@
       <c r="E44" s="5">
         <v>0</v>
       </c>
+      <c r="F44" s="6"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -4211,6 +4228,7 @@
       <c r="E45" s="5">
         <v>0</v>
       </c>
+      <c r="F45" s="6"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -4228,6 +4246,7 @@
       <c r="E46" s="5">
         <v>0</v>
       </c>
+      <c r="F46" s="6"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -4245,6 +4264,7 @@
       <c r="E47" s="5">
         <v>0</v>
       </c>
+      <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
@@ -4262,6 +4282,7 @@
       <c r="E48" s="5">
         <v>0</v>
       </c>
+      <c r="F48" s="6"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
@@ -4279,6 +4300,7 @@
       <c r="E49" s="5">
         <v>0</v>
       </c>
+      <c r="F49" s="6"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
@@ -4296,6 +4318,7 @@
       <c r="E50" s="5">
         <v>0</v>
       </c>
+      <c r="F50" s="6"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
@@ -4313,6 +4336,7 @@
       <c r="E51" s="5">
         <v>0</v>
       </c>
+      <c r="F51" s="6"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
@@ -4330,6 +4354,7 @@
       <c r="E52" s="5">
         <v>0</v>
       </c>
+      <c r="F52" s="6"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
@@ -4347,6 +4372,7 @@
       <c r="E53" s="5">
         <v>0</v>
       </c>
+      <c r="F53" s="6"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
@@ -4364,6 +4390,7 @@
       <c r="E54" s="5">
         <v>0</v>
       </c>
+      <c r="F54" s="6"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -4381,6 +4408,7 @@
       <c r="E55" s="5">
         <v>0</v>
       </c>
+      <c r="F55" s="6"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -4398,6 +4426,7 @@
       <c r="E56" s="5">
         <v>0</v>
       </c>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -4415,6 +4444,7 @@
       <c r="E57" s="5">
         <v>0</v>
       </c>
+      <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -4432,6 +4462,7 @@
       <c r="E58" s="5">
         <v>0</v>
       </c>
+      <c r="F58" s="6"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
@@ -4469,6 +4500,7 @@
       <c r="E60" s="5">
         <v>0</v>
       </c>
+      <c r="F60" s="6"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
@@ -4486,6 +4518,7 @@
       <c r="E61" s="5">
         <v>0</v>
       </c>
+      <c r="F61" s="6"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
@@ -4503,6 +4536,7 @@
       <c r="E62" s="5">
         <v>0</v>
       </c>
+      <c r="F62" s="6"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
@@ -4520,6 +4554,7 @@
       <c r="E63" s="5">
         <v>0</v>
       </c>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
@@ -4537,8 +4572,9 @@
       <c r="E64" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4554,8 +4590,9 @@
       <c r="E65" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4571,8 +4608,9 @@
       <c r="E66" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4588,8 +4626,9 @@
       <c r="E67" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4605,8 +4644,9 @@
       <c r="E68" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4622,8 +4662,9 @@
       <c r="E69" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4639,8 +4680,9 @@
       <c r="E70" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4656,8 +4698,9 @@
       <c r="E71" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4673,8 +4716,9 @@
       <c r="E72" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4690,8 +4734,9 @@
       <c r="E73" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4707,8 +4752,9 @@
       <c r="E74" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4724,8 +4770,9 @@
       <c r="E75" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4741,8 +4788,9 @@
       <c r="E76" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4758,8 +4806,9 @@
       <c r="E77" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4775,8 +4824,9 @@
       <c r="E78" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4792,8 +4842,9 @@
       <c r="E79" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4809,8 +4860,9 @@
       <c r="E80" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4826,8 +4878,9 @@
       <c r="E81" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81" s="6"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4843,8 +4896,9 @@
       <c r="E82" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4860,8 +4914,9 @@
       <c r="E83" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4877,8 +4932,9 @@
       <c r="E84" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84" s="6"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4894,8 +4950,9 @@
       <c r="E85" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85" s="6"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4911,8 +4968,9 @@
       <c r="E86" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86" s="6"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4928,8 +4986,9 @@
       <c r="E87" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87" s="6"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4945,8 +5004,9 @@
       <c r="E88" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88" s="6"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4962,8 +5022,9 @@
       <c r="E89" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4979,8 +5040,9 @@
       <c r="E90" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4996,8 +5058,9 @@
       <c r="E91" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91" s="6"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5013,8 +5076,9 @@
       <c r="E92" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92" s="6"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5030,8 +5094,9 @@
       <c r="E93" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5047,8 +5112,9 @@
       <c r="E94" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94" s="6"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5064,8 +5130,9 @@
       <c r="E95" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95" s="6"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5081,8 +5148,9 @@
       <c r="E96" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96" s="6"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5098,8 +5166,9 @@
       <c r="E97" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97" s="6"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5115,8 +5184,9 @@
       <c r="E98" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98" s="6"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5132,8 +5202,9 @@
       <c r="E99" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99" s="6"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5149,8 +5220,9 @@
       <c r="E100" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100" s="6"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5166,8 +5238,9 @@
       <c r="E101" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F101" s="6"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5183,8 +5256,9 @@
       <c r="E102" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F102" s="6"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5200,8 +5274,9 @@
       <c r="E103" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F103" s="6"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5217,8 +5292,9 @@
       <c r="E104" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F104" s="6"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5234,8 +5310,9 @@
       <c r="E105" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F105" s="6"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5251,8 +5328,9 @@
       <c r="E106" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F106" s="6"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5268,8 +5346,9 @@
       <c r="E107" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F107" s="6"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5285,8 +5364,9 @@
       <c r="E108" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F108" s="6"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5302,8 +5382,9 @@
       <c r="E109" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F109" s="6"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5319,8 +5400,9 @@
       <c r="E110" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F110" s="6"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5336,8 +5418,9 @@
       <c r="E111" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F111" s="6"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5353,8 +5436,9 @@
       <c r="E112" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F112" s="6"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5370,8 +5454,9 @@
       <c r="E113" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F113" s="6"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5387,8 +5472,9 @@
       <c r="E114" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F114" s="6"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5404,8 +5490,9 @@
       <c r="E115" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F115" s="6"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5421,8 +5508,9 @@
       <c r="E116" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F116" s="6"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5438,8 +5526,9 @@
       <c r="E117" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F117" s="6"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5455,8 +5544,9 @@
       <c r="E118" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F118" s="6"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5472,8 +5562,9 @@
       <c r="E119" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F119" s="6"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5489,8 +5580,9 @@
       <c r="E120" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F120" s="6"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5506,8 +5598,9 @@
       <c r="E121" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F121" s="6"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5523,8 +5616,9 @@
       <c r="E122" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F122" s="6"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5540,8 +5634,9 @@
       <c r="E123" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F123" s="6"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5557,8 +5652,9 @@
       <c r="E124" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F124" s="6"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5574,8 +5670,9 @@
       <c r="E125" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F125" s="6"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5591,8 +5688,9 @@
       <c r="E126" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F126" s="6"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5608,8 +5706,9 @@
       <c r="E127" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F127" s="6"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5625,8 +5724,9 @@
       <c r="E128" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F128" s="6"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5642,8 +5742,9 @@
       <c r="E129" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F129" s="6"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5659,8 +5760,9 @@
       <c r="E130" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F130" s="6"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5676,8 +5778,9 @@
       <c r="E131" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F131" s="6"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5693,8 +5796,9 @@
       <c r="E132" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F132" s="6"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5710,8 +5814,9 @@
       <c r="E133" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F133" s="6"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5727,8 +5832,9 @@
       <c r="E134" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F134" s="6"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5744,8 +5850,9 @@
       <c r="E135" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F135" s="6"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5761,8 +5868,9 @@
       <c r="E136" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F136" s="6"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5778,8 +5886,9 @@
       <c r="E137" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F137" s="6"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5795,8 +5904,9 @@
       <c r="E138" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F138" s="6"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5812,8 +5922,9 @@
       <c r="E139" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F139" s="6"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5829,8 +5940,9 @@
       <c r="E140" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F140" s="6"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5846,8 +5958,9 @@
       <c r="E141" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F141" s="6"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5863,8 +5976,9 @@
       <c r="E142" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F142" s="6"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5880,8 +5994,9 @@
       <c r="E143" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F143" s="6"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5897,6 +6012,7 @@
       <c r="E144" s="5">
         <v>0</v>
       </c>
+      <c r="F144" s="6"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
@@ -5914,6 +6030,7 @@
       <c r="E145" s="5">
         <v>0</v>
       </c>
+      <c r="F145" s="6"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
@@ -5931,6 +6048,7 @@
       <c r="E146" s="5">
         <v>0</v>
       </c>
+      <c r="F146" s="6"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
@@ -5948,6 +6066,7 @@
       <c r="E147" s="5">
         <v>0</v>
       </c>
+      <c r="F147" s="6"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
@@ -5965,6 +6084,7 @@
       <c r="E148" s="5">
         <v>0</v>
       </c>
+      <c r="F148" s="6"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
@@ -5982,6 +6102,7 @@
       <c r="E149" s="5">
         <v>0</v>
       </c>
+      <c r="F149" s="6"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
@@ -5999,6 +6120,7 @@
       <c r="E150" s="5">
         <v>0</v>
       </c>
+      <c r="F150" s="6"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
@@ -6016,6 +6138,7 @@
       <c r="E151" s="5">
         <v>0</v>
       </c>
+      <c r="F151" s="6"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
@@ -6053,6 +6176,7 @@
       <c r="E153" s="5">
         <v>0</v>
       </c>
+      <c r="F153" s="6"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
@@ -6090,6 +6214,7 @@
       <c r="E155" s="5">
         <v>0</v>
       </c>
+      <c r="F155" s="6"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
@@ -6107,6 +6232,7 @@
       <c r="E156" s="5">
         <v>0</v>
       </c>
+      <c r="F156" s="6"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
@@ -6124,6 +6250,7 @@
       <c r="E157" s="5">
         <v>0</v>
       </c>
+      <c r="F157" s="6"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
@@ -6141,6 +6268,7 @@
       <c r="E158" s="5">
         <v>0</v>
       </c>
+      <c r="F158" s="6"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
@@ -6158,6 +6286,7 @@
       <c r="E159" s="5">
         <v>0</v>
       </c>
+      <c r="F159" s="6"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
@@ -6175,8 +6304,9 @@
       <c r="E160" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F160" s="6"/>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6192,8 +6322,9 @@
       <c r="E161" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F161" s="6"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6209,8 +6340,9 @@
       <c r="E162" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F162" s="6"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6226,8 +6358,9 @@
       <c r="E163" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F163" s="6"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6243,8 +6376,9 @@
       <c r="E164" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F164" s="6"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6260,8 +6394,9 @@
       <c r="E165" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F165" s="6"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6277,8 +6412,9 @@
       <c r="E166" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F166" s="6"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6294,8 +6430,9 @@
       <c r="E167" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F167" s="6"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6311,8 +6448,9 @@
       <c r="E168" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F168" s="6"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6328,8 +6466,9 @@
       <c r="E169" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F169" s="6"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6345,8 +6484,9 @@
       <c r="E170" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F170" s="6"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6362,8 +6502,9 @@
       <c r="E171" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F171" s="6"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6379,8 +6520,9 @@
       <c r="E172" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F172" s="6"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6396,8 +6538,9 @@
       <c r="E173" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F173" s="6"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6413,8 +6556,9 @@
       <c r="E174" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F174" s="6"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6430,8 +6574,9 @@
       <c r="E175" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F175" s="6"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -6447,8 +6592,9 @@
       <c r="E176" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F176" s="6"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
@@ -6464,8 +6610,9 @@
       <c r="E177" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F177" s="6"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6481,8 +6628,9 @@
       <c r="E178" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F178" s="6"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6498,8 +6646,9 @@
       <c r="E179" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F179" s="6"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -6515,8 +6664,9 @@
       <c r="E180" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F180" s="6"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -6532,8 +6682,9 @@
       <c r="E181" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F181" s="6"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -6549,8 +6700,9 @@
       <c r="E182" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F182" s="6"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -6566,8 +6718,9 @@
       <c r="E183" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F183" s="6"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -6583,8 +6736,9 @@
       <c r="E184" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F184" s="6"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
@@ -6600,8 +6754,9 @@
       <c r="E185" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F185" s="6"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
@@ -6617,8 +6772,9 @@
       <c r="E186" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F186" s="6"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
@@ -6634,8 +6790,9 @@
       <c r="E187" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F187" s="6"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
@@ -6651,8 +6808,9 @@
       <c r="E188" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F188" s="6"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
@@ -6668,8 +6826,9 @@
       <c r="E189" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F189" s="6"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
@@ -6685,8 +6844,9 @@
       <c r="E190" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F190" s="6"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
@@ -6702,8 +6862,9 @@
       <c r="E191" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F191" s="6"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6719,6 +6880,7 @@
       <c r="E192" s="5">
         <v>0</v>
       </c>
+      <c r="F192" s="6"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193">
@@ -6736,6 +6898,7 @@
       <c r="E193" s="5">
         <v>0</v>
       </c>
+      <c r="F193" s="6"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194">
@@ -6753,6 +6916,7 @@
       <c r="E194" s="5">
         <v>0</v>
       </c>
+      <c r="F194" s="6"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195">
@@ -6770,6 +6934,7 @@
       <c r="E195" s="5">
         <v>0</v>
       </c>
+      <c r="F195" s="6"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196">
@@ -6787,6 +6952,7 @@
       <c r="E196" s="5">
         <v>0</v>
       </c>
+      <c r="F196" s="6"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197">
@@ -6804,6 +6970,7 @@
       <c r="E197" s="5">
         <v>0</v>
       </c>
+      <c r="F197" s="6"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198">
@@ -6821,6 +6988,7 @@
       <c r="E198" s="5">
         <v>0</v>
       </c>
+      <c r="F198" s="6"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199">
@@ -6838,6 +7006,7 @@
       <c r="E199" s="5">
         <v>0</v>
       </c>
+      <c r="F199" s="6"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200">
@@ -6875,6 +7044,7 @@
       <c r="E201" s="5">
         <v>0</v>
       </c>
+      <c r="F201" s="6"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202">
@@ -6892,6 +7062,7 @@
       <c r="E202" s="5">
         <v>0</v>
       </c>
+      <c r="F202" s="6"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203">
@@ -6909,6 +7080,7 @@
       <c r="E203" s="5">
         <v>0</v>
       </c>
+      <c r="F203" s="6"/>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204">
@@ -6926,6 +7098,7 @@
       <c r="E204" s="5">
         <v>0</v>
       </c>
+      <c r="F204" s="6"/>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205">
@@ -6943,6 +7116,7 @@
       <c r="E205" s="5">
         <v>0</v>
       </c>
+      <c r="F205" s="6"/>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206">
@@ -6960,6 +7134,7 @@
       <c r="E206" s="5">
         <v>0</v>
       </c>
+      <c r="F206" s="6"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207">
@@ -6977,6 +7152,7 @@
       <c r="E207" s="5">
         <v>0</v>
       </c>
+      <c r="F207" s="6"/>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208">
@@ -6994,8 +7170,9 @@
       <c r="E208" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F208" s="6"/>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
@@ -7011,8 +7188,9 @@
       <c r="E209" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F209" s="6"/>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
@@ -7028,8 +7206,9 @@
       <c r="E210" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F210" s="6"/>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
@@ -7045,8 +7224,9 @@
       <c r="E211" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F211" s="6"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
@@ -7062,8 +7242,9 @@
       <c r="E212" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F212" s="6"/>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
@@ -7079,8 +7260,9 @@
       <c r="E213" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F213" s="6"/>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
@@ -7096,8 +7278,9 @@
       <c r="E214" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F214" s="6"/>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
@@ -7113,8 +7296,9 @@
       <c r="E215" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F215" s="6"/>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
@@ -7130,8 +7314,9 @@
       <c r="E216" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F216" s="6"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
@@ -7147,8 +7332,9 @@
       <c r="E217" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F217" s="6"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
@@ -7164,8 +7350,9 @@
       <c r="E218" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F218" s="6"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
@@ -7181,8 +7368,9 @@
       <c r="E219" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F219" s="6"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
@@ -7198,8 +7386,9 @@
       <c r="E220" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F220" s="6"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
@@ -7215,8 +7404,9 @@
       <c r="E221" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F221" s="6"/>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
@@ -7232,8 +7422,9 @@
       <c r="E222" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F222" s="6"/>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
@@ -7249,8 +7440,9 @@
       <c r="E223" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F223" s="6"/>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
@@ -7266,6 +7458,7 @@
       <c r="E224" s="5">
         <v>0</v>
       </c>
+      <c r="F224" s="6"/>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225">
@@ -7283,6 +7476,7 @@
       <c r="E225" s="5">
         <v>0</v>
       </c>
+      <c r="F225" s="6"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226">
@@ -7320,6 +7514,7 @@
       <c r="E227" s="5">
         <v>0</v>
       </c>
+      <c r="F227" s="6"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228">
@@ -7337,6 +7532,7 @@
       <c r="E228" s="5">
         <v>0</v>
       </c>
+      <c r="F228" s="6"/>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229">
@@ -7354,6 +7550,7 @@
       <c r="E229" s="5">
         <v>0</v>
       </c>
+      <c r="F229" s="6"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230">
@@ -7371,6 +7568,7 @@
       <c r="E230" s="5">
         <v>0</v>
       </c>
+      <c r="F230" s="6"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231">
@@ -7388,6 +7586,7 @@
       <c r="E231" s="5">
         <v>0</v>
       </c>
+      <c r="F231" s="6"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232">
@@ -7405,6 +7604,7 @@
       <c r="E232" s="5">
         <v>0</v>
       </c>
+      <c r="F232" s="6"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233">
@@ -7422,6 +7622,7 @@
       <c r="E233" s="5">
         <v>0</v>
       </c>
+      <c r="F233" s="6"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234">
@@ -7439,6 +7640,7 @@
       <c r="E234" s="5">
         <v>0</v>
       </c>
+      <c r="F234" s="6"/>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235">
@@ -7456,6 +7658,7 @@
       <c r="E235" s="5">
         <v>0</v>
       </c>
+      <c r="F235" s="6"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A236">
@@ -7473,6 +7676,7 @@
       <c r="E236" s="5">
         <v>0</v>
       </c>
+      <c r="F236" s="6"/>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237">
@@ -7490,6 +7694,7 @@
       <c r="E237" s="5">
         <v>0</v>
       </c>
+      <c r="F237" s="6"/>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238">
@@ -7507,6 +7712,7 @@
       <c r="E238" s="5">
         <v>0</v>
       </c>
+      <c r="F238" s="6"/>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239">
@@ -7524,6 +7730,7 @@
       <c r="E239" s="5">
         <v>0</v>
       </c>
+      <c r="F239" s="6"/>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240">
@@ -7541,8 +7748,9 @@
       <c r="E240" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F240" s="6"/>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>240</v>
       </c>
@@ -7558,8 +7766,9 @@
       <c r="E241" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F241" s="6"/>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>241</v>
       </c>
@@ -7575,8 +7784,9 @@
       <c r="E242" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F242" s="6"/>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>242</v>
       </c>
@@ -7592,8 +7802,9 @@
       <c r="E243" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F243" s="6"/>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>243</v>
       </c>
@@ -7609,8 +7820,9 @@
       <c r="E244" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F244" s="6"/>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>244</v>
       </c>
@@ -7626,8 +7838,9 @@
       <c r="E245" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F245" s="6"/>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>245</v>
       </c>
@@ -7643,8 +7856,9 @@
       <c r="E246" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F246" s="6"/>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>246</v>
       </c>
@@ -7660,8 +7874,9 @@
       <c r="E247" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F247" s="6"/>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>247</v>
       </c>
@@ -7677,8 +7892,9 @@
       <c r="E248" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F248" s="6"/>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>248</v>
       </c>
@@ -7694,8 +7910,9 @@
       <c r="E249" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F249" s="6"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>249</v>
       </c>
@@ -7711,8 +7928,9 @@
       <c r="E250" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F250" s="6"/>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>250</v>
       </c>
@@ -7728,8 +7946,9 @@
       <c r="E251" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F251" s="6"/>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>251</v>
       </c>
@@ -7745,8 +7964,9 @@
       <c r="E252" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F252" s="6"/>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>252</v>
       </c>
@@ -7762,8 +7982,9 @@
       <c r="E253" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F253" s="6"/>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>253</v>
       </c>
@@ -7779,8 +8000,9 @@
       <c r="E254" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F254" s="6"/>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>254</v>
       </c>
@@ -7796,8 +8018,9 @@
       <c r="E255" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F255" s="6"/>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>255</v>
       </c>
@@ -7813,8 +8036,9 @@
       <c r="E256" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F256" s="6"/>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>256</v>
       </c>
@@ -7830,8 +8054,9 @@
       <c r="E257" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F257" s="6"/>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>257</v>
       </c>
@@ -7847,8 +8072,9 @@
       <c r="E258" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F258" s="6"/>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>258</v>
       </c>
@@ -7864,8 +8090,9 @@
       <c r="E259" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F259" s="6"/>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>259</v>
       </c>
@@ -7881,8 +8108,9 @@
       <c r="E260" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F260" s="6"/>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>260</v>
       </c>
@@ -7898,8 +8126,9 @@
       <c r="E261" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F261" s="6"/>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>261</v>
       </c>
@@ -7915,8 +8144,9 @@
       <c r="E262" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F262" s="6"/>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>262</v>
       </c>
@@ -7932,8 +8162,9 @@
       <c r="E263" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F263" s="6"/>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>263</v>
       </c>
@@ -7949,8 +8180,9 @@
       <c r="E264" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F264" s="6"/>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>264</v>
       </c>
@@ -7966,8 +8198,9 @@
       <c r="E265" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F265" s="6"/>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>265</v>
       </c>
@@ -7983,8 +8216,9 @@
       <c r="E266" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F266" s="6"/>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>266</v>
       </c>
@@ -8000,8 +8234,9 @@
       <c r="E267" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F267" s="6"/>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>267</v>
       </c>
@@ -8017,8 +8252,9 @@
       <c r="E268" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F268" s="6"/>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>268</v>
       </c>
@@ -8034,8 +8270,9 @@
       <c r="E269" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F269" s="6"/>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>269</v>
       </c>
@@ -8051,8 +8288,9 @@
       <c r="E270" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F270" s="6"/>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>270</v>
       </c>
@@ -8068,8 +8306,9 @@
       <c r="E271" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F271" s="6"/>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>271</v>
       </c>
@@ -8085,6 +8324,7 @@
       <c r="E272" s="5">
         <v>0</v>
       </c>
+      <c r="F272" s="6"/>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A273">
@@ -8102,6 +8342,7 @@
       <c r="E273" s="5">
         <v>0</v>
       </c>
+      <c r="F273" s="6"/>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A274">
@@ -8119,6 +8360,7 @@
       <c r="E274" s="5">
         <v>0</v>
       </c>
+      <c r="F274" s="6"/>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A275">
@@ -8136,6 +8378,7 @@
       <c r="E275" s="5">
         <v>0</v>
       </c>
+      <c r="F275" s="6"/>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A276">
@@ -8153,6 +8396,7 @@
       <c r="E276" s="5">
         <v>0</v>
       </c>
+      <c r="F276" s="6"/>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A277">
@@ -8170,6 +8414,7 @@
       <c r="E277" s="5">
         <v>0</v>
       </c>
+      <c r="F277" s="6"/>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A278">
@@ -8187,6 +8432,7 @@
       <c r="E278" s="5">
         <v>0</v>
       </c>
+      <c r="F278" s="6"/>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A279">
@@ -8264,6 +8510,7 @@
       <c r="E282" s="5">
         <v>0</v>
       </c>
+      <c r="F282" s="6"/>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A283">
@@ -8281,6 +8528,7 @@
       <c r="E283" s="5">
         <v>0</v>
       </c>
+      <c r="F283" s="6"/>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A284">
@@ -8298,6 +8546,7 @@
       <c r="E284" s="5">
         <v>0</v>
       </c>
+      <c r="F284" s="6"/>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A285">
@@ -8315,6 +8564,7 @@
       <c r="E285" s="5">
         <v>0</v>
       </c>
+      <c r="F285" s="6"/>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A286">
@@ -8332,6 +8582,7 @@
       <c r="E286" s="5">
         <v>0</v>
       </c>
+      <c r="F286" s="6"/>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A287">
@@ -8349,6 +8600,7 @@
       <c r="E287" s="5">
         <v>0</v>
       </c>
+      <c r="F287" s="6"/>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A288">
@@ -8366,6 +8618,7 @@
       <c r="E288" s="5">
         <v>0</v>
       </c>
+      <c r="F288" s="6"/>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A289">
@@ -8383,6 +8636,7 @@
       <c r="E289" s="5">
         <v>0</v>
       </c>
+      <c r="F289" s="6"/>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A290">
@@ -8400,6 +8654,7 @@
       <c r="E290" s="5">
         <v>0</v>
       </c>
+      <c r="F290" s="6"/>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A291">
@@ -8417,6 +8672,7 @@
       <c r="E291" s="5">
         <v>0</v>
       </c>
+      <c r="F291" s="6"/>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A292">
@@ -8454,6 +8710,7 @@
       <c r="E293" s="5">
         <v>0</v>
       </c>
+      <c r="F293" s="6"/>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A294">
@@ -8471,6 +8728,7 @@
       <c r="E294" s="5">
         <v>0</v>
       </c>
+      <c r="F294" s="6"/>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A295">
@@ -8488,6 +8746,7 @@
       <c r="E295" s="5">
         <v>0</v>
       </c>
+      <c r="F295" s="6"/>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A296">
@@ -8525,6 +8784,7 @@
       <c r="E297" s="5">
         <v>0</v>
       </c>
+      <c r="F297" s="6"/>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A298">
@@ -8542,6 +8802,7 @@
       <c r="E298" s="5">
         <v>0</v>
       </c>
+      <c r="F298" s="6"/>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A299">
@@ -8559,6 +8820,7 @@
       <c r="E299" s="5">
         <v>0</v>
       </c>
+      <c r="F299" s="6"/>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A300">
@@ -8576,6 +8838,7 @@
       <c r="E300" s="5">
         <v>0</v>
       </c>
+      <c r="F300" s="6"/>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A301">
@@ -8593,6 +8856,7 @@
       <c r="E301" s="5">
         <v>0</v>
       </c>
+      <c r="F301" s="6"/>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A302">
@@ -8610,6 +8874,7 @@
       <c r="E302" s="5">
         <v>0</v>
       </c>
+      <c r="F302" s="6"/>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A303">
@@ -8627,6 +8892,7 @@
       <c r="E303" s="5">
         <v>0</v>
       </c>
+      <c r="F303" s="6"/>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A304">
@@ -8644,6 +8910,7 @@
       <c r="E304" s="5">
         <v>0</v>
       </c>
+      <c r="F304" s="6"/>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A305">
@@ -8661,6 +8928,7 @@
       <c r="E305" s="5">
         <v>0</v>
       </c>
+      <c r="F305" s="6"/>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A306">
@@ -8678,6 +8946,7 @@
       <c r="E306" s="5">
         <v>0</v>
       </c>
+      <c r="F306" s="6"/>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A307">
@@ -8695,6 +8964,7 @@
       <c r="E307" s="5">
         <v>0</v>
       </c>
+      <c r="F307" s="6"/>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A308">
@@ -8712,6 +8982,7 @@
       <c r="E308" s="5">
         <v>0</v>
       </c>
+      <c r="F308" s="6"/>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A309">
@@ -8729,6 +9000,7 @@
       <c r="E309" s="5">
         <v>0</v>
       </c>
+      <c r="F309" s="6"/>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A310">
@@ -8746,6 +9018,7 @@
       <c r="E310" s="5">
         <v>0</v>
       </c>
+      <c r="F310" s="6"/>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A311">
@@ -8763,6 +9036,7 @@
       <c r="E311" s="5">
         <v>0</v>
       </c>
+      <c r="F311" s="6"/>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A312">
@@ -8780,6 +9054,7 @@
       <c r="E312" s="5">
         <v>0</v>
       </c>
+      <c r="F312" s="6"/>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A313">
@@ -8797,6 +9072,7 @@
       <c r="E313" s="5">
         <v>0</v>
       </c>
+      <c r="F313" s="6"/>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A314">
@@ -8814,6 +9090,7 @@
       <c r="E314" s="5">
         <v>0</v>
       </c>
+      <c r="F314" s="6"/>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A315">
@@ -8851,6 +9128,7 @@
       <c r="E316" s="5">
         <v>0</v>
       </c>
+      <c r="F316" s="6"/>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A317">
@@ -8868,6 +9146,7 @@
       <c r="E317" s="5">
         <v>0</v>
       </c>
+      <c r="F317" s="6"/>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A318">
@@ -8885,6 +9164,7 @@
       <c r="E318" s="5">
         <v>0</v>
       </c>
+      <c r="F318" s="6"/>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A319">
@@ -8922,6 +9202,7 @@
       <c r="E320" s="5">
         <v>0</v>
       </c>
+      <c r="F320" s="6"/>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A321">
@@ -8939,6 +9220,7 @@
       <c r="E321" s="5">
         <v>0</v>
       </c>
+      <c r="F321" s="6"/>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A322">
@@ -8956,6 +9238,7 @@
       <c r="E322" s="5">
         <v>0</v>
       </c>
+      <c r="F322" s="6"/>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A323">
@@ -8973,6 +9256,7 @@
       <c r="E323" s="5">
         <v>0</v>
       </c>
+      <c r="F323" s="6"/>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A324">
@@ -8990,6 +9274,7 @@
       <c r="E324" s="5">
         <v>0</v>
       </c>
+      <c r="F324" s="6"/>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A325">
@@ -9007,6 +9292,7 @@
       <c r="E325" s="5">
         <v>0</v>
       </c>
+      <c r="F325" s="6"/>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A326">
@@ -9024,6 +9310,7 @@
       <c r="E326" s="5">
         <v>0</v>
       </c>
+      <c r="F326" s="6"/>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A327">
@@ -9041,6 +9328,7 @@
       <c r="E327" s="5">
         <v>0</v>
       </c>
+      <c r="F327" s="6"/>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A328">
@@ -9058,6 +9346,7 @@
       <c r="E328" s="5">
         <v>0</v>
       </c>
+      <c r="F328" s="6"/>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A329">
@@ -9075,6 +9364,7 @@
       <c r="E329" s="5">
         <v>0</v>
       </c>
+      <c r="F329" s="6"/>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A330">
@@ -9092,6 +9382,7 @@
       <c r="E330" s="5">
         <v>0</v>
       </c>
+      <c r="F330" s="6"/>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A331">
@@ -9109,6 +9400,7 @@
       <c r="E331" s="5">
         <v>0</v>
       </c>
+      <c r="F331" s="6"/>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A332">
@@ -9146,6 +9438,7 @@
       <c r="E333" s="5">
         <v>0</v>
       </c>
+      <c r="F333" s="6"/>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A334">
@@ -9163,6 +9456,7 @@
       <c r="E334" s="5">
         <v>0</v>
       </c>
+      <c r="F334" s="6"/>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A335">
@@ -9180,6 +9474,7 @@
       <c r="E335" s="5">
         <v>0</v>
       </c>
+      <c r="F335" s="6"/>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A336">
@@ -9197,6 +9492,7 @@
       <c r="E336" s="5">
         <v>0</v>
       </c>
+      <c r="F336" s="6"/>
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A337">
@@ -9214,6 +9510,7 @@
       <c r="E337" s="5">
         <v>0</v>
       </c>
+      <c r="F337" s="6"/>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A338">
@@ -9251,6 +9548,7 @@
       <c r="E339" s="5">
         <v>0</v>
       </c>
+      <c r="F339" s="6"/>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A340">
@@ -9268,6 +9566,7 @@
       <c r="E340" s="5">
         <v>0</v>
       </c>
+      <c r="F340" s="6"/>
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A341">
@@ -9285,6 +9584,7 @@
       <c r="E341" s="5">
         <v>0</v>
       </c>
+      <c r="F341" s="6"/>
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A342">
@@ -9302,6 +9602,7 @@
       <c r="E342" s="5">
         <v>0</v>
       </c>
+      <c r="F342" s="6"/>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A343">
@@ -9319,6 +9620,7 @@
       <c r="E343" s="5">
         <v>0</v>
       </c>
+      <c r="F343" s="6"/>
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A344">
@@ -9336,6 +9638,7 @@
       <c r="E344" s="5">
         <v>0</v>
       </c>
+      <c r="F344" s="6"/>
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A345">
@@ -9353,6 +9656,7 @@
       <c r="E345" s="5">
         <v>0</v>
       </c>
+      <c r="F345" s="6"/>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A346">
@@ -9370,6 +9674,7 @@
       <c r="E346" s="5">
         <v>0</v>
       </c>
+      <c r="F346" s="6"/>
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A347">
@@ -9387,6 +9692,7 @@
       <c r="E347" s="5">
         <v>0</v>
       </c>
+      <c r="F347" s="6"/>
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A348">
@@ -9404,6 +9710,7 @@
       <c r="E348" s="5">
         <v>0</v>
       </c>
+      <c r="F348" s="6"/>
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A349">
@@ -9421,6 +9728,7 @@
       <c r="E349" s="5">
         <v>0</v>
       </c>
+      <c r="F349" s="6"/>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A350">
@@ -9438,6 +9746,7 @@
       <c r="E350" s="5">
         <v>0</v>
       </c>
+      <c r="F350" s="6"/>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A351">
@@ -9455,6 +9764,7 @@
       <c r="E351" s="5">
         <v>0</v>
       </c>
+      <c r="F351" s="6"/>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A352">
@@ -9472,8 +9782,9 @@
       <c r="E352" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F352" s="6"/>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>352</v>
       </c>
@@ -9489,8 +9800,9 @@
       <c r="E353" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F353" s="6"/>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>353</v>
       </c>
@@ -9506,8 +9818,9 @@
       <c r="E354" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F354" s="6"/>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>354</v>
       </c>
@@ -9523,8 +9836,9 @@
       <c r="E355" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F355" s="6"/>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>355</v>
       </c>
@@ -9540,8 +9854,9 @@
       <c r="E356" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F356" s="6"/>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>356</v>
       </c>
@@ -9557,8 +9872,9 @@
       <c r="E357" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F357" s="6"/>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>357</v>
       </c>
@@ -9574,8 +9890,9 @@
       <c r="E358" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F358" s="6"/>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>358</v>
       </c>
@@ -9591,8 +9908,9 @@
       <c r="E359" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F359" s="6"/>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>359</v>
       </c>
@@ -9608,8 +9926,9 @@
       <c r="E360" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F360" s="6"/>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>360</v>
       </c>
@@ -9625,8 +9944,9 @@
       <c r="E361" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F361" s="6"/>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>361</v>
       </c>
@@ -9642,8 +9962,9 @@
       <c r="E362" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F362" s="6"/>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>362</v>
       </c>
@@ -9659,8 +9980,9 @@
       <c r="E363" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F363" s="6"/>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>363</v>
       </c>
@@ -9676,8 +9998,9 @@
       <c r="E364" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F364" s="6"/>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>364</v>
       </c>
@@ -9693,8 +10016,9 @@
       <c r="E365" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F365" s="6"/>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>365</v>
       </c>
@@ -9710,8 +10034,9 @@
       <c r="E366" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F366" s="6"/>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>366</v>
       </c>
@@ -9727,8 +10052,9 @@
       <c r="E367" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F367" s="6"/>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>367</v>
       </c>
@@ -9744,8 +10070,9 @@
       <c r="E368" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F368" s="6"/>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>368</v>
       </c>
@@ -9761,8 +10088,9 @@
       <c r="E369" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F369" s="6"/>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>369</v>
       </c>
@@ -9778,8 +10106,9 @@
       <c r="E370" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F370" s="6"/>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>370</v>
       </c>
@@ -9795,8 +10124,9 @@
       <c r="E371" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F371" s="6"/>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>371</v>
       </c>
@@ -9812,8 +10142,9 @@
       <c r="E372" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F372" s="6"/>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>372</v>
       </c>
@@ -9829,8 +10160,9 @@
       <c r="E373" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F373" s="6"/>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>373</v>
       </c>
@@ -9846,8 +10178,9 @@
       <c r="E374" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F374" s="6"/>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>374</v>
       </c>
@@ -9863,8 +10196,9 @@
       <c r="E375" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F375" s="6"/>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>375</v>
       </c>
@@ -9880,8 +10214,9 @@
       <c r="E376" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F376" s="6"/>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>376</v>
       </c>
@@ -9897,8 +10232,9 @@
       <c r="E377" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F377" s="6"/>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>377</v>
       </c>
@@ -9914,8 +10250,9 @@
       <c r="E378" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F378" s="6"/>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>378</v>
       </c>
@@ -9931,8 +10268,9 @@
       <c r="E379" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F379" s="6"/>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>379</v>
       </c>
@@ -9948,8 +10286,9 @@
       <c r="E380" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F380" s="6"/>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>380</v>
       </c>
@@ -9965,8 +10304,9 @@
       <c r="E381" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F381" s="6"/>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>381</v>
       </c>
@@ -9982,8 +10322,9 @@
       <c r="E382" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F382" s="6"/>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>382</v>
       </c>
@@ -9999,8 +10340,9 @@
       <c r="E383" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F383" s="6"/>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>383</v>
       </c>
@@ -10016,6 +10358,7 @@
       <c r="E384" s="5">
         <v>0</v>
       </c>
+      <c r="F384" s="6"/>
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A385">
@@ -10033,6 +10376,7 @@
       <c r="E385" s="5">
         <v>0</v>
       </c>
+      <c r="F385" s="6"/>
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A386">
@@ -10050,6 +10394,7 @@
       <c r="E386" s="5">
         <v>0</v>
       </c>
+      <c r="F386" s="6"/>
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A387">
@@ -10067,6 +10412,7 @@
       <c r="E387" s="5">
         <v>0</v>
       </c>
+      <c r="F387" s="6"/>
     </row>
     <row r="388" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A388">
@@ -10084,6 +10430,7 @@
       <c r="E388" s="5">
         <v>0</v>
       </c>
+      <c r="F388" s="6"/>
     </row>
     <row r="389" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A389">
@@ -10101,6 +10448,7 @@
       <c r="E389" s="5">
         <v>0</v>
       </c>
+      <c r="F389" s="6"/>
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A390">
@@ -10118,6 +10466,7 @@
       <c r="E390" s="5">
         <v>0</v>
       </c>
+      <c r="F390" s="6"/>
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A391">
@@ -10135,6 +10484,7 @@
       <c r="E391" s="5">
         <v>0</v>
       </c>
+      <c r="F391" s="6"/>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A392">
@@ -10152,6 +10502,7 @@
       <c r="E392" s="5">
         <v>0</v>
       </c>
+      <c r="F392" s="6"/>
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A393">
@@ -10169,6 +10520,7 @@
       <c r="E393" s="5">
         <v>0</v>
       </c>
+      <c r="F393" s="6"/>
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A394">
@@ -10186,6 +10538,7 @@
       <c r="E394" s="5">
         <v>0</v>
       </c>
+      <c r="F394" s="6"/>
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A395">
@@ -10203,6 +10556,7 @@
       <c r="E395" s="5">
         <v>0</v>
       </c>
+      <c r="F395" s="6"/>
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A396">
@@ -10220,6 +10574,7 @@
       <c r="E396" s="5">
         <v>0</v>
       </c>
+      <c r="F396" s="6"/>
     </row>
     <row r="397" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A397">
@@ -10257,6 +10612,7 @@
       <c r="E398" s="5">
         <v>0</v>
       </c>
+      <c r="F398" s="6"/>
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A399">
@@ -10274,6 +10630,7 @@
       <c r="E399" s="5">
         <v>0</v>
       </c>
+      <c r="F399" s="6"/>
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A400">
@@ -10291,6 +10648,7 @@
       <c r="E400" s="5">
         <v>0</v>
       </c>
+      <c r="F400" s="6"/>
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A401">
@@ -10311,6 +10669,16 @@
       <c r="F401" s="6" t="s">
         <v>813</v>
       </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D402" s="5"/>
+      <c r="E402" s="5"/>
+      <c r="F402" s="6"/>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D403" s="5"/>
+      <c r="E403" s="5"/>
+      <c r="F403" s="6"/>
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D404" s="5">
@@ -10321,9 +10689,10 @@
         <f>SUM(E2:E401)</f>
         <v>30</v>
       </c>
+      <c r="F404" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1 B1">
+  <conditionalFormatting sqref="B1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10331,7 +10700,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>